<commit_message>
added bank display on slot machine, lucky cat and gitignore file. GREAT JOB SUEYLAN!
</commit_message>
<xml_diff>
--- a/Casino Lotten/Casino Lotten Files/Info Player spreedshet.xlsx
+++ b/Casino Lotten/Casino Lotten Files/Info Player spreedshet.xlsx
@@ -1,41 +1,90 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FrancescoFilotto\Documents\Meine-Programmier-Projekte\Casino Lotten\Casino Lotten Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D0F0F2-5107-4C65-AFB8-9EACDF4171D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="UserInfo" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="UserInfo" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Bank acount</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Sueylan</t>
+  </si>
+  <si>
+    <t>Spieler 1</t>
+  </si>
+  <si>
+    <t>xvy</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Hax</t>
+  </si>
+  <si>
+    <t>heli</t>
+  </si>
+  <si>
+    <t>1134</t>
+  </si>
+  <si>
+    <t>francesco</t>
+  </si>
+  <si>
+    <t>0000</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF0070C0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF0070C0"/>
-      <sz val="16"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -97,95 +146,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -505,99 +495,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="50.77734375" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="50.796875" defaultRowHeight="13.8"/>
   <cols>
-    <col width="150.77734375" customWidth="1" min="4" max="4"/>
+    <col min="4" max="4" width="150.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="49.8" customHeight="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Username</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>Password</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Bank acount</t>
-        </is>
-      </c>
-      <c r="D1" s="4" t="inlineStr">
-        <is>
-          <t>Comment</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Sueylan</t>
-        </is>
-      </c>
-      <c r="B2" s="5" t="n">
+    <row r="1" spans="1:4" ht="49.8" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="5">
         <v>42</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>980</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Spieler 1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>xvy</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
         <v>900</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Max</t>
-        </is>
-      </c>
-      <c r="B4" s="5" t="n">
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5">
         <v>123</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>1200</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Hax</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
         <v>42</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>1060</v>
       </c>
     </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>810</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added bank display on slot machine and lucky cat
</commit_message>
<xml_diff>
--- a/Casino Lotten/Casino Lotten Files/Info Player spreedshet.xlsx
+++ b/Casino Lotten/Casino Lotten Files/Info Player spreedshet.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="UserInfo" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UserInfo" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -115,7 +115,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -510,15 +510,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="50.77734375" defaultRowHeight="14.4" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="50.796875" defaultRowHeight="13.8" outlineLevelCol="0"/>
   <cols>
-    <col width="150.77734375" customWidth="1" min="4" max="4"/>
+    <col width="150.796875" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="49.8" customHeight="1">
@@ -595,6 +595,36 @@
       </c>
       <c r="C5" t="n">
         <v>1060</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>heli</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1134</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>999998999999950</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>francesco</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0000</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1010</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last update before push
</commit_message>
<xml_diff>
--- a/Casino Lotten/Casino Lotten Files/Info Player spreedshet.xlsx
+++ b/Casino Lotten/Casino Lotten Files/Info Player spreedshet.xlsx
@@ -1,90 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FrancescoFilotto\Documents\Meine-Programmier-Projekte\Casino Lotten\Casino Lotten Files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D0F0F2-5107-4C65-AFB8-9EACDF4171D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="UserInfo" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="UserInfo" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Bank acount</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Sueylan</t>
-  </si>
-  <si>
-    <t>Spieler 1</t>
-  </si>
-  <si>
-    <t>xvy</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Hax</t>
-  </si>
-  <si>
-    <t>heli</t>
-  </si>
-  <si>
-    <t>1134</t>
-  </si>
-  <si>
-    <t>francesco</t>
-  </si>
-  <si>
-    <t>0000</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF0070C0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <b val="1"/>
+      <color rgb="FF0070C0"/>
+      <sz val="16"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -146,36 +97,95 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -495,99 +505,129 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.796875" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="50.796875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="4" max="4" width="150.796875" customWidth="1"/>
+    <col width="150.796875" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="49.8" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
+    <row r="1" ht="49.8" customHeight="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Username</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Password</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Bank acount</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Comment</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="5">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Sueylan</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="n">
         <v>42</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>980</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Spieler 1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>xvy</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Max</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="n">
         <v>123</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>1200</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hax</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>42</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="n">
         <v>1060</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>heli</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1134</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
-        <v>810</v>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>francesco</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0000</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>960</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>